<commit_message>
First commit, added counter to mineProject.js
</commit_message>
<xml_diff>
--- a/config/moonshot_ccdi_projects_all.xlsx
+++ b/config/moonshot_ccdi_projects_all.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuw5\Documents\GitHub\INS-ETL\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deforgeac/Documents/projects/INS/repos/INS-ETL/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E431AF21-E3ED-4719-AA3E-2CF00CDFB978}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A424E2-959A-4B46-B1B1-F8E49BA4DF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="285" yWindow="510" windowWidth="28800" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38120" yWindow="500" windowWidth="37500" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="projects" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="465">
   <si>
     <t>2021</t>
   </si>
@@ -711,6 +711,723 @@
   </si>
   <si>
     <t>Contract</t>
+  </si>
+  <si>
+    <t>U01CA224766</t>
+  </si>
+  <si>
+    <t>R01CA226776</t>
+  </si>
+  <si>
+    <t>U01CA247548</t>
+  </si>
+  <si>
+    <t>U01CA232826</t>
+  </si>
+  <si>
+    <t>U01CA250554</t>
+  </si>
+  <si>
+    <t>U01CA224182</t>
+  </si>
+  <si>
+    <t>R01CA230275</t>
+  </si>
+  <si>
+    <t>U01CA254832</t>
+  </si>
+  <si>
+    <t>U01CA224146</t>
+  </si>
+  <si>
+    <t>U01CA233169</t>
+  </si>
+  <si>
+    <t>U01CA233100</t>
+  </si>
+  <si>
+    <t>U01DK124165</t>
+  </si>
+  <si>
+    <t>U01CA247576</t>
+  </si>
+  <si>
+    <t>R01CA204314</t>
+  </si>
+  <si>
+    <t>U01CA250549</t>
+  </si>
+  <si>
+    <t>UH3CA233314</t>
+  </si>
+  <si>
+    <t>UH3CA233229</t>
+  </si>
+  <si>
+    <t>U01CA232758</t>
+  </si>
+  <si>
+    <t>R01CA203923</t>
+  </si>
+  <si>
+    <t>U24CA252977</t>
+  </si>
+  <si>
+    <t>U01AI156189</t>
+  </si>
+  <si>
+    <t>U01CA233074</t>
+  </si>
+  <si>
+    <t>UH3CA233251</t>
+  </si>
+  <si>
+    <t>U01DE028227</t>
+  </si>
+  <si>
+    <t>U01CA233097</t>
+  </si>
+  <si>
+    <t>U01CA223976</t>
+  </si>
+  <si>
+    <t>R01CA249467</t>
+  </si>
+  <si>
+    <t>R01CA249501</t>
+  </si>
+  <si>
+    <t>R01CA204915</t>
+  </si>
+  <si>
+    <t>U01CA224175</t>
+  </si>
+  <si>
+    <t>U01CA164973</t>
+  </si>
+  <si>
+    <t>U24CA224020</t>
+  </si>
+  <si>
+    <t>U01CA224160</t>
+  </si>
+  <si>
+    <t>U24CA224067</t>
+  </si>
+  <si>
+    <t>U01DE028233</t>
+  </si>
+  <si>
+    <t>P50CA244688</t>
+  </si>
+  <si>
+    <t>R01CA176745</t>
+  </si>
+  <si>
+    <t>R01CA249460</t>
+  </si>
+  <si>
+    <t>U01CA231776</t>
+  </si>
+  <si>
+    <t>U01CA233078</t>
+  </si>
+  <si>
+    <t>U01CA224348</t>
+  </si>
+  <si>
+    <t>R01CA231011</t>
+  </si>
+  <si>
+    <t>R37CA230617</t>
+  </si>
+  <si>
+    <t>R01CA197363</t>
+  </si>
+  <si>
+    <t>R01CA175397</t>
+  </si>
+  <si>
+    <t>R01CA215034</t>
+  </si>
+  <si>
+    <t>U01AA027681</t>
+  </si>
+  <si>
+    <t>U01CA224166</t>
+  </si>
+  <si>
+    <t>U01CA233084</t>
+  </si>
+  <si>
+    <t>R01CA211723</t>
+  </si>
+  <si>
+    <t>U01CA217885</t>
+  </si>
+  <si>
+    <t>U01CA233056</t>
+  </si>
+  <si>
+    <t>P50CA244289</t>
+  </si>
+  <si>
+    <t>U01CA233102</t>
+  </si>
+  <si>
+    <t>UM1CA154967</t>
+  </si>
+  <si>
+    <t>R01CA214669</t>
+  </si>
+  <si>
+    <t>U01CA224151</t>
+  </si>
+  <si>
+    <t>R01CA214530</t>
+  </si>
+  <si>
+    <t>U01CA233046</t>
+  </si>
+  <si>
+    <t>U01CA239258</t>
+  </si>
+  <si>
+    <t>U01CA224145</t>
+  </si>
+  <si>
+    <t>R01CA218155</t>
+  </si>
+  <si>
+    <t>P50CA244690</t>
+  </si>
+  <si>
+    <t>R01CA210259</t>
+  </si>
+  <si>
+    <t>U01CA224193</t>
+  </si>
+  <si>
+    <t>U2CCA233303</t>
+  </si>
+  <si>
+    <t>U54CA224081</t>
+  </si>
+  <si>
+    <t>U01CA233167</t>
+  </si>
+  <si>
+    <t>R01CA229164</t>
+  </si>
+  <si>
+    <t>UH3CA233282</t>
+  </si>
+  <si>
+    <t>U24CA180996</t>
+  </si>
+  <si>
+    <t>R01CA210440</t>
+  </si>
+  <si>
+    <t>P50CA244693</t>
+  </si>
+  <si>
+    <t>U54CA224019</t>
+  </si>
+  <si>
+    <t>R01CA124633</t>
+  </si>
+  <si>
+    <t>R01CA204396</t>
+  </si>
+  <si>
+    <t>U24CA180803</t>
+  </si>
+  <si>
+    <t>U2CCA233195</t>
+  </si>
+  <si>
+    <t>R01CA205426</t>
+  </si>
+  <si>
+    <t>P50CA244432</t>
+  </si>
+  <si>
+    <t>U2CCA233284</t>
+  </si>
+  <si>
+    <t>R01CA163915</t>
+  </si>
+  <si>
+    <t>U54CA224079</t>
+  </si>
+  <si>
+    <t>P01CA210944</t>
+  </si>
+  <si>
+    <t>R01CA160495</t>
+  </si>
+  <si>
+    <t>U54CA224068</t>
+  </si>
+  <si>
+    <t>U2CCA233280</t>
+  </si>
+  <si>
+    <t>P50CA244433</t>
+  </si>
+  <si>
+    <t>U2CCA233285</t>
+  </si>
+  <si>
+    <t>U01CA244291</t>
+  </si>
+  <si>
+    <t>U54CA243125</t>
+  </si>
+  <si>
+    <t>UG3CA244697</t>
+  </si>
+  <si>
+    <t>U2CCA233291</t>
+  </si>
+  <si>
+    <t>UM1CA233035</t>
+  </si>
+  <si>
+    <t>U24CA232979</t>
+  </si>
+  <si>
+    <t>U2CCA233254</t>
+  </si>
+  <si>
+    <t>U01CA244452</t>
+  </si>
+  <si>
+    <t>P50CA244431</t>
+  </si>
+  <si>
+    <t>U19CA214253</t>
+  </si>
+  <si>
+    <t>U54CA224070</t>
+  </si>
+  <si>
+    <t>U54CA224018</t>
+  </si>
+  <si>
+    <t>U54CA224083</t>
+  </si>
+  <si>
+    <t>U54CA224076</t>
+  </si>
+  <si>
+    <t>U54CA233223</t>
+  </si>
+  <si>
+    <t>U54CA231638</t>
+  </si>
+  <si>
+    <t>U01DE029255</t>
+  </si>
+  <si>
+    <t>U54CA224065</t>
+  </si>
+  <si>
+    <t>U54CA209978</t>
+  </si>
+  <si>
+    <t>P01CA214278</t>
+  </si>
+  <si>
+    <t>U54CA232568</t>
+  </si>
+  <si>
+    <t>U54CA231637</t>
+  </si>
+  <si>
+    <t>U24CA209923</t>
+  </si>
+  <si>
+    <t>U54CA244438</t>
+  </si>
+  <si>
+    <t>P50CA186786</t>
+  </si>
+  <si>
+    <t>P01CA154303</t>
+  </si>
+  <si>
+    <t>U54CA232561</t>
+  </si>
+  <si>
+    <t>P01CA155258</t>
+  </si>
+  <si>
+    <t>R01CA121118</t>
+  </si>
+  <si>
+    <t>P50CA174521</t>
+  </si>
+  <si>
+    <t>R01CA208205</t>
+  </si>
+  <si>
+    <t>UG3CA244687</t>
+  </si>
+  <si>
+    <t>U24CA210985</t>
+  </si>
+  <si>
+    <t>R01CA221290</t>
+  </si>
+  <si>
+    <t>U24CA210999</t>
+  </si>
+  <si>
+    <t>U24CA209851</t>
+  </si>
+  <si>
+    <t>U24CA194215</t>
+  </si>
+  <si>
+    <t>R01CA099326</t>
+  </si>
+  <si>
+    <t>R01CA143971</t>
+  </si>
+  <si>
+    <t>U01CA232563</t>
+  </si>
+  <si>
+    <t>U2CCA233262</t>
+  </si>
+  <si>
+    <t>U01CA232491</t>
+  </si>
+  <si>
+    <t>R44CA217528</t>
+  </si>
+  <si>
+    <t>R01CA211913</t>
+  </si>
+  <si>
+    <t>U2CCA233238</t>
+  </si>
+  <si>
+    <t>U24CA233243</t>
+  </si>
+  <si>
+    <t>U54CA233306</t>
+  </si>
+  <si>
+    <t>U54CA244711</t>
+  </si>
+  <si>
+    <t>U54CA243126</t>
+  </si>
+  <si>
+    <t>P50CA098258</t>
+  </si>
+  <si>
+    <t>U54CA243124</t>
+  </si>
+  <si>
+    <t>U54CA231630</t>
+  </si>
+  <si>
+    <t>R01CA213102</t>
+  </si>
+  <si>
+    <t>U01CA244314</t>
+  </si>
+  <si>
+    <t>R33CA212806</t>
+  </si>
+  <si>
+    <t>R01CA205967</t>
+  </si>
+  <si>
+    <t>R01CA188900</t>
+  </si>
+  <si>
+    <t>R01CA211927</t>
+  </si>
+  <si>
+    <t>R01CA211339</t>
+  </si>
+  <si>
+    <t>U01CA199334</t>
+  </si>
+  <si>
+    <t>R01CA204136</t>
+  </si>
+  <si>
+    <t>R42CA183376</t>
+  </si>
+  <si>
+    <t>U01DE029188</t>
+  </si>
+  <si>
+    <t>UG3CA244298</t>
+  </si>
+  <si>
+    <t>U01CA233085</t>
+  </si>
+  <si>
+    <t>R01CA218306</t>
+  </si>
+  <si>
+    <t>U54CA244719</t>
+  </si>
+  <si>
+    <t>R01CA207445</t>
+  </si>
+  <si>
+    <t>R01CA194511</t>
+  </si>
+  <si>
+    <t>R01CA187532</t>
+  </si>
+  <si>
+    <t>R01CA131261</t>
+  </si>
+  <si>
+    <t>R01CA192914</t>
+  </si>
+  <si>
+    <t>U24CA199347</t>
+  </si>
+  <si>
+    <t>R33CA202881</t>
+  </si>
+  <si>
+    <t>U54CA244726</t>
+  </si>
+  <si>
+    <t>U24CA180924</t>
+  </si>
+  <si>
+    <t>R44CA199826</t>
+  </si>
+  <si>
+    <t>R33CA206949</t>
+  </si>
+  <si>
+    <t>U01CA232361</t>
+  </si>
+  <si>
+    <t>U24CA233032</t>
+  </si>
+  <si>
+    <t>R21CA220398</t>
+  </si>
+  <si>
+    <t>UG3CA233314</t>
+  </si>
+  <si>
+    <t>U01CA233096</t>
+  </si>
+  <si>
+    <t>U01CA232836</t>
+  </si>
+  <si>
+    <t>U01CA232795</t>
+  </si>
+  <si>
+    <t>U54CA231649</t>
+  </si>
+  <si>
+    <t>R00CA181500</t>
+  </si>
+  <si>
+    <t>UM1CA233080</t>
+  </si>
+  <si>
+    <t>U01CA232486</t>
+  </si>
+  <si>
+    <t>UG3CA233282</t>
+  </si>
+  <si>
+    <t>U54CA231641</t>
+  </si>
+  <si>
+    <t>R21CA202875</t>
+  </si>
+  <si>
+    <t>R01CA196658</t>
+  </si>
+  <si>
+    <t>R21CA215968</t>
+  </si>
+  <si>
+    <t>UG3CA233229</t>
+  </si>
+  <si>
+    <t>UM1CA233033</t>
+  </si>
+  <si>
+    <t>UG3CA233251</t>
+  </si>
+  <si>
+    <t>U01CA232488</t>
+  </si>
+  <si>
+    <t>U54CA231652</t>
+  </si>
+  <si>
+    <t>U2CCA233311</t>
+  </si>
+  <si>
+    <t>U01CA209936</t>
+  </si>
+  <si>
+    <t>R01CA181204</t>
+  </si>
+  <si>
+    <t>R01CA180279</t>
+  </si>
+  <si>
+    <t>R44CA221624</t>
+  </si>
+  <si>
+    <t>R01CA187076</t>
+  </si>
+  <si>
+    <t>R01CA182543</t>
+  </si>
+  <si>
+    <t>R33CA192980</t>
+  </si>
+  <si>
+    <t>R33CA191245</t>
+  </si>
+  <si>
+    <t>R01AR070234</t>
+  </si>
+  <si>
+    <t>R01AI124487</t>
+  </si>
+  <si>
+    <t>R01AI109294</t>
+  </si>
+  <si>
+    <t>R01AR050026</t>
+  </si>
+  <si>
+    <t>R01AI084880</t>
+  </si>
+  <si>
+    <t>P01AI118688</t>
+  </si>
+  <si>
+    <t>R01AI018697</t>
+  </si>
+  <si>
+    <t>U24CA224316</t>
+  </si>
+  <si>
+    <t>R33CA225248</t>
+  </si>
+  <si>
+    <t>R33CA225291</t>
+  </si>
+  <si>
+    <t>R33CA225400</t>
+  </si>
+  <si>
+    <t>R33CA225344</t>
+  </si>
+  <si>
+    <t>R33CA225323</t>
+  </si>
+  <si>
+    <t>U24CA224319</t>
+  </si>
+  <si>
+    <t>R33CA225310</t>
+  </si>
+  <si>
+    <t>R21CA191179</t>
+  </si>
+  <si>
+    <t>R33CA225296</t>
+  </si>
+  <si>
+    <t>R33CA225281</t>
+  </si>
+  <si>
+    <t>U24CA224285</t>
+  </si>
+  <si>
+    <t>U24CA224309</t>
+  </si>
+  <si>
+    <t>R33CA225328</t>
+  </si>
+  <si>
+    <t>U24CA224331</t>
+  </si>
+  <si>
+    <t>R41CA213678</t>
+  </si>
+  <si>
+    <t>R21 CA215968</t>
+  </si>
+  <si>
+    <t>U01 CA224182</t>
+  </si>
+  <si>
+    <t>U01 CA224166–01</t>
+  </si>
+  <si>
+    <t>U01 CA233169</t>
+  </si>
+  <si>
+    <t>1UG3CA244687</t>
+  </si>
+  <si>
+    <t>U54 CA231638</t>
+  </si>
+  <si>
+    <t>U54 CA243124</t>
+  </si>
+  <si>
+    <t>U24 CA252977</t>
+  </si>
+  <si>
+    <t>U01 CA232836</t>
+  </si>
+  <si>
+    <t>5U19CA214253</t>
+  </si>
+  <si>
+    <t>U01 CA232795</t>
+  </si>
+  <si>
+    <t>R01 CA249501 and R01CA249501-01</t>
+  </si>
+  <si>
+    <t>1P50 CA244693-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P50CA244432 and P50 CA244432 </t>
+  </si>
+  <si>
+    <t>R01 CA249467</t>
+  </si>
+  <si>
+    <t>1U54CA224070-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U54CA244726 </t>
+  </si>
+  <si>
+    <t>Moonshot of interest</t>
+  </si>
+  <si>
+    <t>Moonshot of interest that break (returns 1 result, isn't scraped)</t>
   </si>
 </sst>
 </file>
@@ -731,7 +1448,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -750,6 +1467,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -763,7 +1486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -774,6 +1497,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1076,21 +1804,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E206"/>
+  <dimension ref="A1:F449"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A161" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A403" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F428" sqref="F428"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="1" max="2" width="33.5" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>167</v>
       </c>
@@ -1107,7 +1835,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>159</v>
       </c>
@@ -1124,7 +1852,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>160</v>
       </c>
@@ -1141,7 +1869,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>128</v>
       </c>
@@ -1158,7 +1886,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>144</v>
       </c>
@@ -1175,7 +1903,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>136</v>
       </c>
@@ -1192,7 +1920,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>135</v>
       </c>
@@ -1209,7 +1937,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>134</v>
       </c>
@@ -1226,7 +1954,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>150</v>
       </c>
@@ -1243,7 +1971,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>130</v>
       </c>
@@ -1260,7 +1988,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>145</v>
       </c>
@@ -1277,7 +2005,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>131</v>
       </c>
@@ -1294,7 +2022,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>133</v>
       </c>
@@ -1311,7 +2039,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>124</v>
       </c>
@@ -1328,7 +2056,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>120</v>
       </c>
@@ -1345,7 +2073,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>140</v>
       </c>
@@ -1362,7 +2090,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>139</v>
       </c>
@@ -1379,7 +2107,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>142</v>
       </c>
@@ -1396,7 +2124,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>127</v>
       </c>
@@ -1413,7 +2141,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>141</v>
       </c>
@@ -1430,7 +2158,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>121</v>
       </c>
@@ -1447,7 +2175,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>147</v>
       </c>
@@ -1464,7 +2192,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>146</v>
       </c>
@@ -1481,7 +2209,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>125</v>
       </c>
@@ -1498,7 +2226,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>149</v>
       </c>
@@ -1515,7 +2243,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>122</v>
       </c>
@@ -1532,7 +2260,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>129</v>
       </c>
@@ -1549,7 +2277,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>132</v>
       </c>
@@ -1566,7 +2294,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>137</v>
       </c>
@@ -1583,7 +2311,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>123</v>
       </c>
@@ -1600,7 +2328,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>126</v>
       </c>
@@ -1617,7 +2345,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>143</v>
       </c>
@@ -1634,7 +2362,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>154</v>
       </c>
@@ -1651,7 +2379,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>151</v>
       </c>
@@ -1668,7 +2396,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>148</v>
       </c>
@@ -1685,7 +2413,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>155</v>
       </c>
@@ -1702,7 +2430,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>153</v>
       </c>
@@ -1719,7 +2447,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>152</v>
       </c>
@@ -1736,7 +2464,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>138</v>
       </c>
@@ -1753,7 +2481,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>156</v>
       </c>
@@ -1770,7 +2498,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>119</v>
       </c>
@@ -1787,7 +2515,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>165</v>
       </c>
@@ -1804,7 +2532,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>164</v>
       </c>
@@ -1821,7 +2549,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>161</v>
       </c>
@@ -1838,7 +2566,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>162</v>
       </c>
@@ -1855,7 +2583,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>158</v>
       </c>
@@ -1872,7 +2600,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>157</v>
       </c>
@@ -1889,7 +2617,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>163</v>
       </c>
@@ -1906,7 +2634,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>100</v>
       </c>
@@ -1923,7 +2651,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>110</v>
       </c>
@@ -1940,7 +2668,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>92</v>
       </c>
@@ -1957,7 +2685,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>59</v>
       </c>
@@ -1974,7 +2702,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>90</v>
       </c>
@@ -1991,7 +2719,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>73</v>
       </c>
@@ -2008,7 +2736,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>97</v>
       </c>
@@ -2025,7 +2753,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>72</v>
       </c>
@@ -2042,7 +2770,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>80</v>
       </c>
@@ -2059,7 +2787,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>89</v>
       </c>
@@ -2076,7 +2804,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>63</v>
       </c>
@@ -2093,7 +2821,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>86</v>
       </c>
@@ -2110,7 +2838,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>76</v>
       </c>
@@ -2127,7 +2855,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>87</v>
       </c>
@@ -2144,7 +2872,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>93</v>
       </c>
@@ -2161,7 +2889,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>77</v>
       </c>
@@ -2178,7 +2906,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>96</v>
       </c>
@@ -2195,7 +2923,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>98</v>
       </c>
@@ -2212,7 +2940,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>79</v>
       </c>
@@ -2229,7 +2957,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>75</v>
       </c>
@@ -2246,7 +2974,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>74</v>
       </c>
@@ -2263,7 +2991,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>68</v>
       </c>
@@ -2280,7 +3008,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>91</v>
       </c>
@@ -2297,7 +3025,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>78</v>
       </c>
@@ -2314,7 +3042,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>62</v>
       </c>
@@ -2331,7 +3059,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>95</v>
       </c>
@@ -2348,7 +3076,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>67</v>
       </c>
@@ -2365,7 +3093,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>99</v>
       </c>
@@ -2382,7 +3110,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>105</v>
       </c>
@@ -2399,7 +3127,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>61</v>
       </c>
@@ -2416,7 +3144,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>109</v>
       </c>
@@ -2433,7 +3161,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>60</v>
       </c>
@@ -2450,7 +3178,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>102</v>
       </c>
@@ -2467,7 +3195,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>108</v>
       </c>
@@ -2484,7 +3212,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>104</v>
       </c>
@@ -2501,7 +3229,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>107</v>
       </c>
@@ -2518,7 +3246,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>106</v>
       </c>
@@ -2535,7 +3263,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>64</v>
       </c>
@@ -2552,7 +3280,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>101</v>
       </c>
@@ -2569,7 +3297,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>103</v>
       </c>
@@ -2586,7 +3314,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>71</v>
       </c>
@@ -2603,7 +3331,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>85</v>
       </c>
@@ -2620,7 +3348,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>82</v>
       </c>
@@ -2637,7 +3365,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>84</v>
       </c>
@@ -2654,7 +3382,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>83</v>
       </c>
@@ -2671,7 +3399,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>66</v>
       </c>
@@ -2688,7 +3416,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>88</v>
       </c>
@@ -2705,7 +3433,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>94</v>
       </c>
@@ -2722,7 +3450,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>58</v>
       </c>
@@ -2739,7 +3467,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>117</v>
       </c>
@@ -2756,7 +3484,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>113</v>
       </c>
@@ -2773,7 +3501,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>111</v>
       </c>
@@ -2790,7 +3518,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>115</v>
       </c>
@@ -2807,7 +3535,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>112</v>
       </c>
@@ -2824,7 +3552,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>114</v>
       </c>
@@ -2841,7 +3569,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>116</v>
       </c>
@@ -2858,7 +3586,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>65</v>
       </c>
@@ -2875,7 +3603,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>70</v>
       </c>
@@ -2892,7 +3620,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>69</v>
       </c>
@@ -2909,7 +3637,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>81</v>
       </c>
@@ -2926,7 +3654,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>37</v>
       </c>
@@ -2943,7 +3671,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>40</v>
       </c>
@@ -2960,7 +3688,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>34</v>
       </c>
@@ -2977,7 +3705,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>22</v>
       </c>
@@ -2994,7 +3722,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>41</v>
       </c>
@@ -3011,7 +3739,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>43</v>
       </c>
@@ -3028,7 +3756,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>55</v>
       </c>
@@ -3045,7 +3773,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>48</v>
       </c>
@@ -3062,7 +3790,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>53</v>
       </c>
@@ -3079,7 +3807,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>51</v>
       </c>
@@ -3096,7 +3824,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>49</v>
       </c>
@@ -3113,7 +3841,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>50</v>
       </c>
@@ -3130,7 +3858,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>26</v>
       </c>
@@ -3147,7 +3875,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>23</v>
       </c>
@@ -3164,7 +3892,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>29</v>
       </c>
@@ -3181,7 +3909,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>31</v>
       </c>
@@ -3198,7 +3926,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>27</v>
       </c>
@@ -3215,7 +3943,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>32</v>
       </c>
@@ -3232,7 +3960,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>38</v>
       </c>
@@ -3249,7 +3977,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>33</v>
       </c>
@@ -3266,7 +3994,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>30</v>
       </c>
@@ -3283,7 +4011,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>54</v>
       </c>
@@ -3300,7 +4028,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>56</v>
       </c>
@@ -3317,7 +4045,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>21</v>
       </c>
@@ -3334,7 +4062,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>45</v>
       </c>
@@ -3351,7 +4079,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>44</v>
       </c>
@@ -3368,7 +4096,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>36</v>
       </c>
@@ -3385,7 +4113,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>39</v>
       </c>
@@ -3402,7 +4130,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>24</v>
       </c>
@@ -3419,7 +4147,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>42</v>
       </c>
@@ -3436,7 +4164,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>46</v>
       </c>
@@ -3453,7 +4181,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>52</v>
       </c>
@@ -3470,7 +4198,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>35</v>
       </c>
@@ -3487,7 +4215,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>28</v>
       </c>
@@ -3504,7 +4232,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>25</v>
       </c>
@@ -3521,7 +4249,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>47</v>
       </c>
@@ -3538,7 +4266,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>11</v>
       </c>
@@ -3555,7 +4283,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>6</v>
       </c>
@@ -3572,7 +4300,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>8</v>
       </c>
@@ -3589,7 +4317,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>7</v>
       </c>
@@ -3606,7 +4334,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>10</v>
       </c>
@@ -3623,7 +4351,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>5</v>
       </c>
@@ -3640,7 +4368,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>15</v>
       </c>
@@ -3657,7 +4385,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>19</v>
       </c>
@@ -3674,7 +4402,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>18</v>
       </c>
@@ -3691,7 +4419,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>14</v>
       </c>
@@ -3708,7 +4436,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>9</v>
       </c>
@@ -3725,7 +4453,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>3</v>
       </c>
@@ -3742,7 +4470,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>12</v>
       </c>
@@ -3759,7 +4487,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>13</v>
       </c>
@@ -3776,7 +4504,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>17</v>
       </c>
@@ -3793,7 +4521,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>16</v>
       </c>
@@ -3810,7 +4538,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>4</v>
       </c>
@@ -3827,7 +4555,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>1</v>
       </c>
@@ -3844,7 +4572,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>185</v>
       </c>
@@ -3861,7 +4589,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>169</v>
       </c>
@@ -3878,7 +4606,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>172</v>
       </c>
@@ -3895,7 +4623,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>170</v>
       </c>
@@ -3912,7 +4640,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>170</v>
       </c>
@@ -3929,7 +4657,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>186</v>
       </c>
@@ -3946,7 +4674,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>187</v>
       </c>
@@ -3963,7 +4691,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>173</v>
       </c>
@@ -3980,7 +4708,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>171</v>
       </c>
@@ -3997,7 +4725,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>168</v>
       </c>
@@ -4014,7 +4742,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>188</v>
       </c>
@@ -4031,7 +4759,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>177</v>
       </c>
@@ -4048,7 +4776,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>179</v>
       </c>
@@ -4065,7 +4793,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>180</v>
       </c>
@@ -4082,7 +4810,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>176</v>
       </c>
@@ -4099,7 +4827,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>175</v>
       </c>
@@ -4116,7 +4844,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>174</v>
       </c>
@@ -4133,7 +4861,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>182</v>
       </c>
@@ -4150,7 +4878,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>181</v>
       </c>
@@ -4167,7 +4895,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>183</v>
       </c>
@@ -4184,7 +4912,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>178</v>
       </c>
@@ -4201,7 +4929,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>189</v>
       </c>
@@ -4218,7 +4946,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>190</v>
       </c>
@@ -4235,7 +4963,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>191</v>
       </c>
@@ -4252,7 +4980,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>192</v>
       </c>
@@ -4269,7 +4997,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>193</v>
       </c>
@@ -4286,7 +5014,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>194</v>
       </c>
@@ -4303,7 +5031,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>195</v>
       </c>
@@ -4320,7 +5048,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>196</v>
       </c>
@@ -4337,7 +5065,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>197</v>
       </c>
@@ -4354,7 +5082,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>198</v>
       </c>
@@ -4371,7 +5099,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>199</v>
       </c>
@@ -4388,7 +5116,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>200</v>
       </c>
@@ -4405,7 +5133,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>201</v>
       </c>
@@ -4422,7 +5150,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>202</v>
       </c>
@@ -4439,7 +5167,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>203</v>
       </c>
@@ -4456,7 +5184,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>204</v>
       </c>
@@ -4473,7 +5201,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>205</v>
       </c>
@@ -4490,7 +5218,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>206</v>
       </c>
@@ -4507,7 +5235,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>185</v>
       </c>
@@ -4524,7 +5252,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>207</v>
       </c>
@@ -4541,7 +5269,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>208</v>
       </c>
@@ -4558,7 +5286,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>188</v>
       </c>
@@ -4575,7 +5303,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>209</v>
       </c>
@@ -4590,6 +5318,1227 @@
       </c>
       <c r="E206" s="7" t="s">
         <v>218</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="F207" s="8" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A253" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A254" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A255" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A256" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A257" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A258" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A259" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A260" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A261" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A262" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A263" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A264" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A265" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A276" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A277" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A278" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A279" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A280" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A281" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A282" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A283" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A284" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A285" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A286" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A287" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A288" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A290" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A291" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A292" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A293" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A294" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A295" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A296" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A297" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A298" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A299" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A300" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A301" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A302" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A303" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A304" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A305" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A306" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A307" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A308" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A309" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A310" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A311" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A312" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A313" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A314" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A315" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A316" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A317" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A318" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A319" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A320" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A321" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A322" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A323" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A324" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A325" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A326" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A327" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A328" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A329" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A330" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A331" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A332" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A333" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A334" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A335" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A336" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A337" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A338" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A339" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A340" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A341" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A342" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A343" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A344" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A345" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A346" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A347" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A348" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A349" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A350" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A351" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A352" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A353" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A354" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A355" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A356" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A357" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A358" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A359" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A360" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A361" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A362" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A363" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A364" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A365" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A366" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A367" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A368" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A369" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A370" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A371" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A372" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A373" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A374" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A375" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A376" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A377" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A378" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A379" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A380" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A381" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A382" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A383" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A384" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A385" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A386" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A387" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A388" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A389" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A390" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A391" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A392" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A393" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A394" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A395" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A396" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A397" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A398" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A399" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A400" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A401" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A402" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A403" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A404" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A405" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A406" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A407" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A408" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A409" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A410" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A411" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A412" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A413" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A414" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A415" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A416" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A417" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A418" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A419" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A420" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A421" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A422" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A423" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A424" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A425" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A426" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A427" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="F427" s="11" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A428" s="12" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A429" s="12" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A430" s="12" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A431" s="12" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A432" s="12" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A433" s="12" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A434" s="12" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A435" s="12" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A436" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A437" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A438" s="12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A439" s="12" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A440" s="12" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A441" s="12" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A442" s="12" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A443" s="12" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A444" s="12" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A445" s="12" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A446" s="12" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A447" s="12" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A448" s="12" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A449" s="12" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented DOM parsing for pages with multiple or single results; need to assure new methodology with ground truth data.
</commit_message>
<xml_diff>
--- a/config/moonshot_ccdi_projects_all.xlsx
+++ b/config/moonshot_ccdi_projects_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deforgeac/Documents/projects/INS/repos/INS-ETL/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A424E2-959A-4B46-B1B1-F8E49BA4DF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB3590E-8681-C54B-BEE6-A39F60513497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38120" yWindow="500" windowWidth="37500" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="467">
   <si>
     <t>2021</t>
   </si>
@@ -1428,6 +1428,12 @@
   </si>
   <si>
     <t>Moonshot of interest that break (returns 1 result, isn't scraped)</t>
+  </si>
+  <si>
+    <t>asdfasdfasdf</t>
+  </si>
+  <si>
+    <t>No results</t>
   </si>
 </sst>
 </file>
@@ -1486,7 +1492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -1502,6 +1508,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1804,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F449"/>
+  <dimension ref="A1:F450"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A403" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F428" sqref="F428"/>
+    <sheetView tabSelected="1" topLeftCell="A404" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C438" sqref="C438"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5324,6 +5332,18 @@
       <c r="A207" s="9" t="s">
         <v>226</v>
       </c>
+      <c r="B207" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C207" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D207" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="E207" s="13" t="s">
+        <v>212</v>
+      </c>
       <c r="F207" s="8" t="s">
         <v>463</v>
       </c>
@@ -6427,117 +6447,152 @@
       <c r="A427" s="10" t="s">
         <v>311</v>
       </c>
+      <c r="B427" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C427" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D427" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="E427" s="14" t="s">
+        <v>212</v>
+      </c>
       <c r="F427" s="11" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="428" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A428" s="12" t="s">
-        <v>446</v>
+      <c r="A428" t="s">
+        <v>465</v>
+      </c>
+      <c r="F428" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="429" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A429" s="12" t="s">
-        <v>257</v>
+        <v>446</v>
       </c>
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A430" s="12" t="s">
-        <v>447</v>
+        <v>257</v>
+      </c>
+      <c r="B430" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C430" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D430" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E430" s="2" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A431" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A432" s="12" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A433" s="12" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A433" s="12" t="s">
+    <row r="434" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A434" s="12" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A434" s="12" t="s">
+    <row r="435" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A435" s="12" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A435" s="12" t="s">
+    <row r="436" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A436" s="12" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A436" s="12" t="s">
+    <row r="437" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A437" s="12" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A437" s="12" t="s">
+    <row r="438" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A438" s="12" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A438" s="12" t="s">
+      <c r="F438" s="11" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A439" s="12" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A439" s="12" t="s">
+    <row r="440" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A440" s="12" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A440" s="12" t="s">
+    <row r="441" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A441" s="12" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A441" s="12" t="s">
+    <row r="442" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A442" s="12" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A442" s="12" t="s">
+    <row r="443" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A443" s="12" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A443" s="12" t="s">
+    <row r="444" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A444" s="12" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A444" s="12" t="s">
+    <row r="445" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A445" s="12" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A445" s="12" t="s">
+    <row r="446" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A446" s="12" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A446" s="12" t="s">
+    <row r="447" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A447" s="12" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A447" s="12" t="s">
+    <row r="448" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A448" s="12" t="s">
         <v>461</v>
-      </c>
-    </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A448" s="12" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A449" s="12" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A450" s="12" t="s">
         <v>261</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented detecting and scraping single page results, plus some minor debugging output.
</commit_message>
<xml_diff>
--- a/config/moonshot_ccdi_projects_all.xlsx
+++ b/config/moonshot_ccdi_projects_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deforgeac/Documents/projects/INS/repos/INS-ETL/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB3590E-8681-C54B-BEE6-A39F60513497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D4B9EB-813B-4F4B-8E61-ED6974E3ACDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38120" yWindow="500" windowWidth="37500" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="453">
   <si>
     <t>2021</t>
   </si>
@@ -1373,74 +1373,32 @@
     <t>R41CA213678</t>
   </si>
   <si>
-    <t>R21 CA215968</t>
-  </si>
-  <si>
-    <t>U01 CA224182</t>
-  </si>
-  <si>
-    <t>U01 CA224166–01</t>
-  </si>
-  <si>
-    <t>U01 CA233169</t>
-  </si>
-  <si>
     <t>1UG3CA244687</t>
   </si>
   <si>
-    <t>U54 CA231638</t>
-  </si>
-  <si>
-    <t>U54 CA243124</t>
-  </si>
-  <si>
-    <t>U24 CA252977</t>
-  </si>
-  <si>
-    <t>U01 CA232836</t>
-  </si>
-  <si>
     <t>5U19CA214253</t>
   </si>
   <si>
-    <t>U01 CA232795</t>
-  </si>
-  <si>
-    <t>R01 CA249501 and R01CA249501-01</t>
-  </si>
-  <si>
-    <t>1P50 CA244693-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P50CA244432 and P50 CA244432 </t>
-  </si>
-  <si>
-    <t>R01 CA249467</t>
-  </si>
-  <si>
-    <t>1U54CA224070-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U54CA244726 </t>
-  </si>
-  <si>
     <t>Moonshot of interest</t>
   </si>
   <si>
     <t>Moonshot of interest that break (returns 1 result, isn't scraped)</t>
   </si>
   <si>
-    <t>asdfasdfasdf</t>
-  </si>
-  <si>
-    <t>No results</t>
+    <t>1U54CA224068</t>
+  </si>
+  <si>
+    <t>1P50CA244693</t>
+  </si>
+  <si>
+    <t>1U54CA224070</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1450,6 +1408,11 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1812,10 +1775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F450"/>
+  <dimension ref="A1:F447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A404" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C438" sqref="C438"/>
+    <sheetView tabSelected="1" topLeftCell="A415" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D446" sqref="D446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5345,7 +5308,7 @@
         <v>212</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
@@ -6460,140 +6423,350 @@
         <v>212</v>
       </c>
       <c r="F427" s="11" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
     </row>
     <row r="428" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A428" t="s">
-        <v>465</v>
-      </c>
-      <c r="F428" t="s">
-        <v>466</v>
+      <c r="A428" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="B428" t="s">
+        <v>224</v>
+      </c>
+      <c r="C428">
+        <v>2018</v>
+      </c>
+      <c r="D428" t="s">
+        <v>219</v>
+      </c>
+      <c r="E428" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="429" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A429" s="12" t="s">
-        <v>446</v>
+        <v>257</v>
+      </c>
+      <c r="B429" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C429" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D429" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E429" s="2" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A430" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="B430" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C430" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D430" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E430" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B430" t="s">
+        <v>224</v>
+      </c>
+      <c r="C430">
+        <v>2017</v>
+      </c>
+      <c r="D430" t="s">
+        <v>219</v>
+      </c>
+      <c r="E430" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A431" s="12" t="s">
-        <v>447</v>
+        <v>273</v>
+      </c>
+      <c r="B431" t="s">
+        <v>224</v>
+      </c>
+      <c r="C431">
+        <v>2017</v>
+      </c>
+      <c r="D431" t="s">
+        <v>219</v>
+      </c>
+      <c r="E431" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A432" s="12" t="s">
-        <v>448</v>
+        <v>235</v>
+      </c>
+      <c r="B432" t="s">
+        <v>224</v>
+      </c>
+      <c r="C432">
+        <v>2018</v>
+      </c>
+      <c r="D432" t="s">
+        <v>219</v>
+      </c>
+      <c r="E432" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="433" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A433" s="12" t="s">
-        <v>449</v>
+        <v>446</v>
+      </c>
+      <c r="B433" t="s">
+        <v>224</v>
+      </c>
+      <c r="C433">
+        <v>2019</v>
+      </c>
+      <c r="D433" t="s">
+        <v>219</v>
+      </c>
+      <c r="E433" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="434" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A434" s="12" t="s">
-        <v>450</v>
+        <v>330</v>
+      </c>
+      <c r="B434" t="s">
+        <v>224</v>
+      </c>
+      <c r="C434">
+        <v>2018</v>
+      </c>
+      <c r="D434" t="s">
+        <v>219</v>
+      </c>
+      <c r="E434" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="435" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A435" s="12" t="s">
-        <v>451</v>
+        <v>365</v>
+      </c>
+      <c r="B435" t="s">
+        <v>224</v>
+      </c>
+      <c r="C435">
+        <v>2019</v>
+      </c>
+      <c r="D435" t="s">
+        <v>219</v>
+      </c>
+      <c r="E435" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="436" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A436" s="12" t="s">
-        <v>452</v>
+        <v>245</v>
+      </c>
+      <c r="B436" t="s">
+        <v>224</v>
+      </c>
+      <c r="C436">
+        <v>2020</v>
+      </c>
+      <c r="D436" t="s">
+        <v>219</v>
+      </c>
+      <c r="E436" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="437" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A437" s="12" t="s">
-        <v>453</v>
+        <v>450</v>
+      </c>
+      <c r="B437" t="s">
+        <v>224</v>
+      </c>
+      <c r="C437" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D437" t="s">
+        <v>219</v>
+      </c>
+      <c r="E437" t="s">
+        <v>212</v>
+      </c>
+      <c r="F437" s="11" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="438" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A438" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="F438" s="11" t="s">
-        <v>464</v>
+        <v>249</v>
+      </c>
+      <c r="B438" t="s">
+        <v>224</v>
+      </c>
+      <c r="C438">
+        <v>2018</v>
+      </c>
+      <c r="D438" t="s">
+        <v>219</v>
+      </c>
+      <c r="E438" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="439" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A439" s="12" t="s">
-        <v>249</v>
+        <v>398</v>
+      </c>
+      <c r="B439" t="s">
+        <v>224</v>
+      </c>
+      <c r="C439">
+        <v>2019</v>
+      </c>
+      <c r="D439" t="s">
+        <v>219</v>
+      </c>
+      <c r="E439" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="440" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A440" s="12" t="s">
-        <v>454</v>
+        <v>447</v>
+      </c>
+      <c r="B440" t="s">
+        <v>224</v>
+      </c>
+      <c r="C440">
+        <v>2019</v>
+      </c>
+      <c r="D440" t="s">
+        <v>219</v>
+      </c>
+      <c r="E440" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="441" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A441" s="12" t="s">
-        <v>455</v>
+        <v>399</v>
+      </c>
+      <c r="B441" t="s">
+        <v>224</v>
+      </c>
+      <c r="C441">
+        <v>2019</v>
+      </c>
+      <c r="D441" t="s">
+        <v>219</v>
+      </c>
+      <c r="E441" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="442" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A442" s="12" t="s">
-        <v>456</v>
+        <v>451</v>
+      </c>
+      <c r="B442" t="s">
+        <v>224</v>
+      </c>
+      <c r="C442">
+        <v>2019</v>
+      </c>
+      <c r="D442" t="s">
+        <v>219</v>
+      </c>
+      <c r="E442" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="443" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A443" s="12" t="s">
-        <v>457</v>
+        <v>305</v>
+      </c>
+      <c r="B443" t="s">
+        <v>224</v>
+      </c>
+      <c r="C443">
+        <v>2019</v>
+      </c>
+      <c r="D443" t="s">
+        <v>219</v>
+      </c>
+      <c r="E443" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="444" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A444" s="12" t="s">
-        <v>458</v>
+        <v>312</v>
+      </c>
+      <c r="B444" t="s">
+        <v>224</v>
+      </c>
+      <c r="C444">
+        <v>2018</v>
+      </c>
+      <c r="D444" t="s">
+        <v>219</v>
+      </c>
+      <c r="E444" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="445" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A445" s="12" t="s">
-        <v>459</v>
+        <v>252</v>
+      </c>
+      <c r="B445" t="s">
+        <v>224</v>
+      </c>
+      <c r="C445">
+        <v>2020</v>
+      </c>
+      <c r="D445" t="s">
+        <v>219</v>
+      </c>
+      <c r="E445" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="446" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A446" s="12" t="s">
-        <v>312</v>
+        <v>452</v>
+      </c>
+      <c r="B446" t="s">
+        <v>224</v>
+      </c>
+      <c r="C446">
+        <v>2017</v>
+      </c>
+      <c r="D446" t="s">
+        <v>219</v>
+      </c>
+      <c r="E446" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="447" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A447" s="12" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A448" s="12" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A449" s="12" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A450" s="12" t="s">
         <v>261</v>
+      </c>
+      <c r="B447" t="s">
+        <v>224</v>
+      </c>
+      <c r="C447">
+        <v>2019</v>
+      </c>
+      <c r="D447" t="s">
+        <v>219</v>
+      </c>
+      <c r="E447" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -6602,6 +6775,7 @@
       <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
These changes generated the most recent presented data.
</commit_message>
<xml_diff>
--- a/config/moonshot_ccdi_projects_all.xlsx
+++ b/config/moonshot_ccdi_projects_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deforgeac/Documents/projects/INS/repos/INS-ETL/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D4B9EB-813B-4F4B-8E61-ED6974E3ACDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10D88A3-FAED-CE4C-A1BB-6BADC3514A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38120" yWindow="500" windowWidth="37500" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="555">
   <si>
     <t>2021</t>
   </si>
@@ -1392,6 +1392,312 @@
   </si>
   <si>
     <t>1U54CA224070</t>
+  </si>
+  <si>
+    <t>3P01AI118688-02S1</t>
+  </si>
+  <si>
+    <t>2P01CA154303-06</t>
+  </si>
+  <si>
+    <t>1P01CA210944-01</t>
+  </si>
+  <si>
+    <t>1P01CA214278-01</t>
+  </si>
+  <si>
+    <t>5P50CA098258-12</t>
+  </si>
+  <si>
+    <t>5P50CA174521-03</t>
+  </si>
+  <si>
+    <t>5P50CA186786-04</t>
+  </si>
+  <si>
+    <t>1P50CA244690-01</t>
+  </si>
+  <si>
+    <t>3R01AI018697-36S1</t>
+  </si>
+  <si>
+    <t>3R01AI084880-07S1</t>
+  </si>
+  <si>
+    <t>3R01AI109294-03S1</t>
+  </si>
+  <si>
+    <t>3R01AI124487-02S1</t>
+  </si>
+  <si>
+    <t>3R01AR050026-12A1S1</t>
+  </si>
+  <si>
+    <t>7R01AR070234-03</t>
+  </si>
+  <si>
+    <t>5R01CA099326-23</t>
+  </si>
+  <si>
+    <t>5R01CA121118-09</t>
+  </si>
+  <si>
+    <t>5R01CA124633-10</t>
+  </si>
+  <si>
+    <t>5R01CA131261-08</t>
+  </si>
+  <si>
+    <t>5R01CA143971-07</t>
+  </si>
+  <si>
+    <t>2R01CA160495-06A1</t>
+  </si>
+  <si>
+    <t>2R01CA163915-06</t>
+  </si>
+  <si>
+    <t>5R01CA175397-05</t>
+  </si>
+  <si>
+    <t>2R01CA176745-07</t>
+  </si>
+  <si>
+    <t>5R01CA180279-04</t>
+  </si>
+  <si>
+    <t>5R01CA181204-05</t>
+  </si>
+  <si>
+    <t>5R01CA182543-05</t>
+  </si>
+  <si>
+    <t>5R01CA187076-04</t>
+  </si>
+  <si>
+    <t>5R01CA187532-03</t>
+  </si>
+  <si>
+    <t>5R01CA188900-03</t>
+  </si>
+  <si>
+    <t>5R01CA192914-03</t>
+  </si>
+  <si>
+    <t>5R01CA194511-03</t>
+  </si>
+  <si>
+    <t>5R01CA196658-02</t>
+  </si>
+  <si>
+    <t>1R01CA197363-01A1</t>
+  </si>
+  <si>
+    <t>5R01CA203923-02</t>
+  </si>
+  <si>
+    <t>5R01CA204136-02</t>
+  </si>
+  <si>
+    <t>5R01CA204314-02</t>
+  </si>
+  <si>
+    <t>5R01CA204396-02</t>
+  </si>
+  <si>
+    <t>3R01CA204915-01A1S1</t>
+  </si>
+  <si>
+    <t>1R01CA205426-01A1</t>
+  </si>
+  <si>
+    <t>5R01CA205967-02</t>
+  </si>
+  <si>
+    <t>1R01CA207445-01A1</t>
+  </si>
+  <si>
+    <t>1R01CA208205-01A1</t>
+  </si>
+  <si>
+    <t>1R01CA210440-01A1</t>
+  </si>
+  <si>
+    <t>1R01CA211339-01A1</t>
+  </si>
+  <si>
+    <t>1R01CA211913-01A1</t>
+  </si>
+  <si>
+    <t>1R01CA211927-01</t>
+  </si>
+  <si>
+    <t>1R01CA213102-01A1</t>
+  </si>
+  <si>
+    <t>1R01CA214530-01</t>
+  </si>
+  <si>
+    <t>1R01CA214669-01A1</t>
+  </si>
+  <si>
+    <t>1R01CA215034-01</t>
+  </si>
+  <si>
+    <t>1R01CA218155-01</t>
+  </si>
+  <si>
+    <t>1R01CA221290-01</t>
+  </si>
+  <si>
+    <t>1R01CA226776-01</t>
+  </si>
+  <si>
+    <t>1R01CA229164-01A1</t>
+  </si>
+  <si>
+    <t>1R01CA230275-01A1</t>
+  </si>
+  <si>
+    <t>1R01CA231011-01A1</t>
+  </si>
+  <si>
+    <t>5R21CA191179-03</t>
+  </si>
+  <si>
+    <t>5R21CA202875-02</t>
+  </si>
+  <si>
+    <t>1R21CA215968-01</t>
+  </si>
+  <si>
+    <t>1R21CA220398-01</t>
+  </si>
+  <si>
+    <t>5R33CA191245-03</t>
+  </si>
+  <si>
+    <t>5R33CA192980-03</t>
+  </si>
+  <si>
+    <t>1R33CA202881-01A1</t>
+  </si>
+  <si>
+    <t>5R33CA206949-02</t>
+  </si>
+  <si>
+    <t>1R33CA212806-01A1</t>
+  </si>
+  <si>
+    <t>1R37CA230617-01A1</t>
+  </si>
+  <si>
+    <t>1R41CA213678-01A1</t>
+  </si>
+  <si>
+    <t>2R42CA183376-02</t>
+  </si>
+  <si>
+    <t>2R44CA199826-02A1</t>
+  </si>
+  <si>
+    <t>1R44CA217528-01A1</t>
+  </si>
+  <si>
+    <t>1R44CA221624-01</t>
+  </si>
+  <si>
+    <t>2U01CA164973-06</t>
+  </si>
+  <si>
+    <t>5U01CA199334-03</t>
+  </si>
+  <si>
+    <t>5U01CA209936-02</t>
+  </si>
+  <si>
+    <t>1U01CA217885-01</t>
+  </si>
+  <si>
+    <t>1U01CA223976-01A1</t>
+  </si>
+  <si>
+    <t>1U01CA224766-01</t>
+  </si>
+  <si>
+    <t>1U01CA231776-01</t>
+  </si>
+  <si>
+    <t>1U01CA250549-01</t>
+  </si>
+  <si>
+    <t>1U01CA250554-01</t>
+  </si>
+  <si>
+    <t>1U01CA254832-01</t>
+  </si>
+  <si>
+    <t>1U19CA214253-01A1</t>
+  </si>
+  <si>
+    <t>5U24CA180803-04</t>
+  </si>
+  <si>
+    <t>5U24CA180924-04</t>
+  </si>
+  <si>
+    <t>5U24CA180996-05</t>
+  </si>
+  <si>
+    <t>5U24CA194215-02</t>
+  </si>
+  <si>
+    <t>5U24CA199347-02</t>
+  </si>
+  <si>
+    <t>5U24CA209851-02</t>
+  </si>
+  <si>
+    <t>5U24CA209923-02</t>
+  </si>
+  <si>
+    <t>5U24CA210985-02</t>
+  </si>
+  <si>
+    <t>5U24CA210999-02</t>
+  </si>
+  <si>
+    <t>1U24CA232979-01</t>
+  </si>
+  <si>
+    <t>1U2CCA233284-01</t>
+  </si>
+  <si>
+    <t>1U2CCA233285-01</t>
+  </si>
+  <si>
+    <t>1U54CA209978-01A1</t>
+  </si>
+  <si>
+    <t>1U54CA224065-01</t>
+  </si>
+  <si>
+    <t>1U54CA224076-01</t>
+  </si>
+  <si>
+    <t>4UH3CA233229-02</t>
+  </si>
+  <si>
+    <t>4UH3CA233251-02</t>
+  </si>
+  <si>
+    <t>4UH3CA233282-02</t>
+  </si>
+  <si>
+    <t>4UH3CA233314-02</t>
+  </si>
+  <si>
+    <t>Moonshot of interest (raw)</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1723,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1442,6 +1748,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1455,7 +1767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -1473,6 +1785,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1775,10 +2089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F447"/>
+  <dimension ref="A1:F667"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A415" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D446" sqref="D446"/>
+    <sheetView tabSelected="1" topLeftCell="A429" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F449" sqref="F449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6769,6 +7083,1109 @@
         <v>212</v>
       </c>
     </row>
+    <row r="448" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A448" s="16" t="s">
+        <v>453</v>
+      </c>
+      <c r="F448" s="15" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A449" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A450" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A451" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A452" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A453" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A454" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A455" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A456" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A457" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A458" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A459" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A460" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A461" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A462" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A463" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A464" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A465" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A466" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A467" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A468" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A469" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A470" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A471" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A472" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A473" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A474" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A475" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A476" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A477" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A478" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A479" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A480" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A481" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A482" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A483" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A484" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A485" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A486" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A487" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A488" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A489" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A490" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A491" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A492" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A493" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A494" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A495" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A496" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A497" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A498" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A499" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A500" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A501" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A502" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A503" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A504" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A505" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A506" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A507" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A508" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A509" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A510" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A511" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A512" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A513" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A514" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A515" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A516" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A517" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A518" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A519" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A520" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A521" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A522" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A523" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A524" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A525" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A526" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A527" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A528" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A529" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A530" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A531" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A532" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A533" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A534" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A535" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A536" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A537" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A538" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A539" s="1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A540" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A541" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A542" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A543" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A544" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A545" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A546" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A547" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A548" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A549" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A550" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A551" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A552" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A553" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A554" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A555" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A556" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A557" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A558" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A559" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A560" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A561" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A562" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A563" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A564" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A565" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A566" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A567" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A568" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A569" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A570" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A571" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A572" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="573" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A573" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A574" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A575" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A576" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A577" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A578" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="579" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A579" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="580" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A580" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="581" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A581" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A582" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A583" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A584" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A585" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A586" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A587" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="588" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A588" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A589" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A590" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A591" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A592" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A593" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A594" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A595" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A596" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A597" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A598" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="599" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A599" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A600" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="601" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A601" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="602" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A602" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="603" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A603" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="604" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A604" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="605" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A605" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="606" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A606" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="607" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A607" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="608" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A608" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="609" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A609" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A610" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="611" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A611" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="612" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A612" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="613" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A613" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="614" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A614" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="615" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A615" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="616" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A616" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="617" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A617" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="618" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A618" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="619" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A619" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="620" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A620" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="621" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A621" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="622" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A622" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="623" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A623" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A624" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="625" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A625" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="626" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A626" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="627" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A627" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="628" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A628" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="629" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A629" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="630" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A630" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="631" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A631" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="632" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A632" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="633" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A633" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="634" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A634" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="635" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A635" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="636" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A636" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="637" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A637" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="638" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A638" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="639" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A639" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="640" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A640" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="641" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A641" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="642" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A642" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="643" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A643" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="644" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A644" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="645" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A645" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="646" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A646" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="647" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A647" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="648" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A648" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="649" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A649" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="650" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A650" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="651" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A651" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="652" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A652" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="653" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A653" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="654" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A654" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="655" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A655" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="656" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A656" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="657" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A657" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="658" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A658" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="659" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A659" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="660" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A660" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="661" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A661" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="662" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A662" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="663" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A663" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="664" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A664" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="665" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A665" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="666" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A666" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="667" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A667" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{054C75E2-536B-45B9-856C-719EA27B3499}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C162">

</xml_diff>